<commit_message>
Hoja con la gráfica de líneas básica
</commit_message>
<xml_diff>
--- a/07/GraficosI.xlsx
+++ b/07/GraficosI.xlsx
@@ -108,6 +108,1013 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HistoricoMundial!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Población mundial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>HistoricoMundial!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1955</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1960</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HistoricoMundial!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>791</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>981</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="#,##0">
+                  <c:v>1262</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="#,##0">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="#,##0">
+                  <c:v>2516</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="#,##0">
+                  <c:v>2751</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="#,##0">
+                  <c:v>3018</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>3335</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>3697</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>4077</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0">
+                  <c:v>4446</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="#,##0">
+                  <c:v>4854</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="#,##0">
+                  <c:v>5259</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="#,##0">
+                  <c:v>5759</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="#,##0">
+                  <c:v>6228</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="#,##0">
+                  <c:v>6574</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="#,##0">
+                  <c:v>6894</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="#,##0">
+                  <c:v>7349</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-952E-4D6C-B97F-65190D1DF59F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="678529976"/>
+        <c:axId val="678528664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="678529976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678528664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="678528664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678529976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,5 +1558,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hoja con distintas formas gráficas
</commit_message>
<xml_diff>
--- a/07/GraficosI.xlsx
+++ b/07/GraficosI.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="8955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HistoricoMundial" sheetId="1" r:id="rId1"/>
     <sheet name="Minigráficos" sheetId="2" r:id="rId2"/>
+    <sheet name="Formas" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Poblacion">Minigráficos!$A$2:$I$226</definedName>
@@ -1997,6 +1998,453 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="14 Cubo"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904875" y="1790700"/>
+          <a:ext cx="1485900" cy="1323975"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
+        </a:blipFill>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="accent1">
+              <a:satMod val="175000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+          <a:outerShdw blurRad="76200" dist="12700" dir="8100000" sy="-23000" kx="800400" algn="br" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="20000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3312702" cy="843693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="13 CuadroTexto"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3200399" y="628650"/>
+          <a:ext cx="3312702" cy="843693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+          <a:reflection blurRad="6350" stA="50000" endA="295" endPos="92000" dist="101600" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="perspectiveContrastingRightFacing"/>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="soft" dir="t">
+              <a:rot lat="0" lon="0" rev="10800000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="27940" h="12700"/>
+            <a:contourClr>
+              <a:srgbClr val="DDDDDD"/>
+            </a:contourClr>
+          </a:sp3d>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="2400" b="1" cap="none" spc="150">
+              <a:ln w="11430"/>
+              <a:solidFill>
+                <a:srgbClr val="F8F8F8"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="25400" algn="tl" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Manual Avanzado</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="2400" b="1" cap="none" spc="150">
+              <a:ln w="11430"/>
+              <a:solidFill>
+                <a:srgbClr val="F8F8F8"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="25400" algn="tl" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="43000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Microsoft  Excel 2016</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 68">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm rot="10800000">
+          <a:off x="5334000" y="3048000"/>
+          <a:ext cx="1352550" cy="1847850"/>
+          <a:chOff x="978" y="61"/>
+          <a:chExt cx="128" cy="192"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="AutoShape 65"/>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="978" y="62"/>
+            <a:ext cx="128" cy="96"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="G0" fmla="+- 5400 0 0"/>
+              <a:gd name="G1" fmla="+- 21600 0 5400"/>
+              <a:gd name="G2" fmla="*/ 5400 1 2"/>
+              <a:gd name="G3" fmla="+- 21600 0 G2"/>
+              <a:gd name="G4" fmla="+/ 5400 21600 2"/>
+              <a:gd name="G5" fmla="+/ G1 0 2"/>
+              <a:gd name="G6" fmla="*/ 21600 21600 5400"/>
+              <a:gd name="G7" fmla="*/ G6 1 2"/>
+              <a:gd name="G8" fmla="+- 21600 0 G7"/>
+              <a:gd name="G9" fmla="*/ 21600 1 2"/>
+              <a:gd name="G10" fmla="+- 5400 0 G9"/>
+              <a:gd name="G11" fmla="?: G10 G8 0"/>
+              <a:gd name="G12" fmla="?: G10 G7 21600"/>
+              <a:gd name="T0" fmla="*/ 18900 w 21600"/>
+              <a:gd name="T1" fmla="*/ 10800 h 21600"/>
+              <a:gd name="T2" fmla="*/ 10800 w 21600"/>
+              <a:gd name="T3" fmla="*/ 21600 h 21600"/>
+              <a:gd name="T4" fmla="*/ 2700 w 21600"/>
+              <a:gd name="T5" fmla="*/ 10800 h 21600"/>
+              <a:gd name="T6" fmla="*/ 10800 w 21600"/>
+              <a:gd name="T7" fmla="*/ 0 h 21600"/>
+              <a:gd name="T8" fmla="*/ 4500 w 21600"/>
+              <a:gd name="T9" fmla="*/ 4500 h 21600"/>
+              <a:gd name="T10" fmla="*/ 17100 w 21600"/>
+              <a:gd name="T11" fmla="*/ 17100 h 21600"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="T0" y="T1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="T2" y="T3"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="T4" y="T5"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="T6" y="T7"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="T8" t="T9" r="T10" b="T11"/>
+            <a:pathLst>
+              <a:path w="21600" h="21600">
+                <a:moveTo>
+                  <a:pt x="0" y="0"/>
+                </a:moveTo>
+                <a:lnTo>
+                  <a:pt x="5400" y="21600"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="16200" y="21600"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="21600" y="0"/>
+                </a:lnTo>
+                <a:close/>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw sy="50000" kx="-2453608" rotWithShape="0">
+              <a:srgbClr val="808080">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="AutoShape 66"/>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="10800000">
+            <a:off x="978" y="157"/>
+            <a:ext cx="128" cy="96"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="G0" fmla="+- 5400 0 0"/>
+              <a:gd name="G1" fmla="+- 21600 0 5400"/>
+              <a:gd name="G2" fmla="*/ 5400 1 2"/>
+              <a:gd name="G3" fmla="+- 21600 0 G2"/>
+              <a:gd name="G4" fmla="+/ 5400 21600 2"/>
+              <a:gd name="G5" fmla="+/ G1 0 2"/>
+              <a:gd name="G6" fmla="*/ 21600 21600 5400"/>
+              <a:gd name="G7" fmla="*/ G6 1 2"/>
+              <a:gd name="G8" fmla="+- 21600 0 G7"/>
+              <a:gd name="G9" fmla="*/ 21600 1 2"/>
+              <a:gd name="G10" fmla="+- 5400 0 G9"/>
+              <a:gd name="G11" fmla="?: G10 G8 0"/>
+              <a:gd name="G12" fmla="?: G10 G7 21600"/>
+              <a:gd name="T0" fmla="*/ 18900 w 21600"/>
+              <a:gd name="T1" fmla="*/ 10800 h 21600"/>
+              <a:gd name="T2" fmla="*/ 10800 w 21600"/>
+              <a:gd name="T3" fmla="*/ 21600 h 21600"/>
+              <a:gd name="T4" fmla="*/ 2700 w 21600"/>
+              <a:gd name="T5" fmla="*/ 10800 h 21600"/>
+              <a:gd name="T6" fmla="*/ 10800 w 21600"/>
+              <a:gd name="T7" fmla="*/ 0 h 21600"/>
+              <a:gd name="T8" fmla="*/ 4500 w 21600"/>
+              <a:gd name="T9" fmla="*/ 4500 h 21600"/>
+              <a:gd name="T10" fmla="*/ 17100 w 21600"/>
+              <a:gd name="T11" fmla="*/ 17100 h 21600"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="T0" y="T1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="T2" y="T3"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="T4" y="T5"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="T6" y="T7"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="T8" t="T9" r="T10" b="T11"/>
+            <a:pathLst>
+              <a:path w="21600" h="21600">
+                <a:moveTo>
+                  <a:pt x="0" y="0"/>
+                </a:moveTo>
+                <a:lnTo>
+                  <a:pt x="5400" y="21600"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="16200" y="21600"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="21600" y="0"/>
+                </a:lnTo>
+                <a:close/>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw sy="50000" kx="-2453608" rotWithShape="0">
+              <a:srgbClr val="808080">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </xdr:spPr>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="AutoShape 67"/>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="994" y="61"/>
+            <a:ext cx="96" cy="96"/>
+          </a:xfrm>
+          <a:prstGeom prst="sun">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 25000"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="9525">
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+          <a:scene3d>
+            <a:camera prst="legacyObliqueTopRight"/>
+            <a:lightRig rig="legacyFlat3" dir="b"/>
+          </a:scene3d>
+          <a:sp3d extrusionH="11100" prstMaterial="legacyMatte">
+            <a:bevelT w="13500" h="13500" prst="angle"/>
+            <a:bevelB w="13500" h="13500" prst="angle"/>
+            <a:extrusionClr>
+              <a:srgbClr val="FFFFFF"/>
+            </a:extrusionClr>
+          </a:sp3d>
+        </xdr:spPr>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -2446,7 +2894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="C59" sqref="C59:F59"/>
     </sheetView>
   </sheetViews>
@@ -9995,4 +10443,19 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>